<commit_message>
New Deposit Test committed
</commit_message>
<xml_diff>
--- a/src/main/java/com/TFBanking/qa/testdata/testData.xlsx
+++ b/src/main/java/com/TFBanking/qa/testdata/testData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasrayeganeh/Desktop/Selenium/exlProject/src/main/java/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasrayeganeh/Desktop/AutomationWebsites 2/UI/src/main/java/com/TFBanking/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581ADE0F-0CD8-A041-8E4E-629C67EF206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1177EB2-557B-C14A-BEA8-BEFCF1F8A7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{24067596-8CEB-EC43-9757-DBBBA15B2F35}"/>
+    <workbookView xWindow="760" yWindow="1240" windowWidth="28040" windowHeight="16100" activeTab="1" xr2:uid="{24067596-8CEB-EC43-9757-DBBBA15B2F35}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="ContactsData" sheetId="5" r:id="rId2"/>
-    <sheet name="DashboardData" sheetId="3" r:id="rId3"/>
-    <sheet name="AddCustomersData" sheetId="2" r:id="rId4"/>
+    <sheet name="NewDepositData" sheetId="6" r:id="rId2"/>
+    <sheet name="ContactsData" sheetId="5" r:id="rId3"/>
+    <sheet name="DashboardData" sheetId="3" r:id="rId4"/>
+    <sheet name="AddCustomersData" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>Password</t>
   </si>
@@ -127,12 +128,6 @@
     <t>Dashboard Header</t>
   </si>
   <si>
-    <t>Login Username</t>
-  </si>
-  <si>
-    <t>Login Password</t>
-  </si>
-  <si>
     <t>Add Contact</t>
   </si>
   <si>
@@ -149,13 +144,112 @@
   </si>
   <si>
     <t>a123-543-</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>abc124</t>
+  </si>
+  <si>
+    <t>Valid/Invalid</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>demo1@techfios.com</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Tags1</t>
+  </si>
+  <si>
+    <t>Tags2</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>Transaction ID: </t>
+  </si>
+  <si>
+    <t>Regular Income</t>
+  </si>
+  <si>
+    <t>Paycheck</t>
+  </si>
+  <si>
+    <t>Stub</t>
+  </si>
+  <si>
+    <t>SEL278</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Selling Software</t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>US747</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
+    <t>2024-04-20</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Debit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,13 +265,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -201,6 +315,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,43 +635,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8107CEBA-10FC-3146-B895-5CEBB7691CBC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{55E3469E-2CF1-074F-9CB8-5163C1FC27CA}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{6E70BD3D-8F1C-D247-B8A9-00F046473BB3}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{6FDF8184-6C91-9B43-90B7-08CECF127A34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C21E082-AF09-A447-AC8C-5286B503B489}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="14.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="14.6640625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBCFF2B-F83C-C840-869D-F38851D646D5}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -567,12 +835,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -580,7 +848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17C444A-7792-2C4F-B1EF-90DA01889364}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -608,11 +876,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F72896-53FB-D84F-9587-783CCDEEC5A0}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="116" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="116" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -634,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -676,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -690,7 +958,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -723,7 +991,7 @@
         <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>